<commit_message>
move button "Open", "Save", "Close", "Filters" to Toolbar. create buttons to change font, size, bold and italics without implementations
</commit_message>
<xml_diff>
--- a/test2.xlsx
+++ b/test2.xlsx
@@ -457,64 +457,64 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="n">
+      <c r="A1" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>123</t>
         </is>
       </c>
-      <c r="C1" t="n">
+      <c r="C1" s="2" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="2" t="inlineStr">
         <is>
           <t>f</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2" s="2" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C2" s="2" t="inlineStr">
         <is>
           <t>afsaf</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" s="2" t="inlineStr">
         <is>
           <t>d</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B3" s="2" t="inlineStr">
         <is>
           <t>wqrw</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C3" s="2" t="inlineStr">
         <is>
           <t>ффф</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
+      <c r="A4" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B4" s="2" t="inlineStr">
         <is>
           <t>sgd</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>a</t>
+      <c r="C4" s="2" t="inlineStr">
+        <is>
+          <t>124</t>
         </is>
       </c>
     </row>
@@ -538,58 +538,58 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="inlineStr">
+      <c r="A1" t="inlineStr">
         <is>
           <t>124</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>a</t>
         </is>
       </c>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>1421</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="B2" s="2" t="inlineStr">
+      <c r="B2" t="inlineStr">
         <is>
           <t>124</t>
         </is>
       </c>
-      <c r="C2" s="2" t="inlineStr">
+      <c r="C2" t="inlineStr">
         <is>
           <t>afasa</t>
         </is>
       </c>
-      <c r="D2" s="2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>ewt</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="C3" s="2" t="inlineStr">
+      <c r="C3" t="inlineStr">
         <is>
           <t>fsgsdg</t>
         </is>
       </c>
-      <c r="D3" s="2" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>1512</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="C4" s="2" t="n">
+      <c r="C4" t="n">
         <v>124121</v>
       </c>
     </row>
     <row r="5">
-      <c r="C5" s="2" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t>sgd</t>
         </is>
@@ -597,7 +597,7 @@
     </row>
     <row r="6"/>
     <row r="7">
-      <c r="D7" s="2" t="inlineStr">
+      <c r="D7" t="inlineStr">
         <is>
           <t>aaaa</t>
         </is>

</xml_diff>

<commit_message>
+ add "help" button with some information + add shortcuts + add bold / italic / size / font name changer + fix some bugs
</commit_message>
<xml_diff>
--- a/test2.xlsx
+++ b/test2.xlsx
@@ -18,7 +18,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="4">
+  <fonts count="32">
     <font>
       <name val="Arial"/>
       <charset val="204"/>
@@ -42,6 +42,187 @@
       <charset val="204"/>
       <family val="0"/>
       <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <charset val="204"/>
+      <family val="2"/>
+      <b val="1"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="1"/>
+      <family val="2"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val=""/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <charset val="204"/>
+      <family val="2"/>
+      <i val="1"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <charset val="204"/>
+      <family val="2"/>
+      <b val="1"/>
+      <i val="1"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <charset val="204"/>
+      <family val="2"/>
+      <i val="1"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <charset val="204"/>
+      <family val="2"/>
+      <i val="1"/>
+      <sz val="7"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <charset val="204"/>
+      <family val="2"/>
+      <sz val="7"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <charset val="204"/>
+      <family val="2"/>
+      <i val="1"/>
+      <sz val="8"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <charset val="204"/>
+      <family val="2"/>
+      <sz val="8"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <charset val="204"/>
+      <family val="2"/>
+      <i val="1"/>
+      <sz val="9"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <charset val="204"/>
+      <family val="2"/>
+      <sz val="9"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <charset val="204"/>
+      <family val="2"/>
+      <i val="1"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <charset val="204"/>
+      <family val="2"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <charset val="204"/>
+      <family val="2"/>
+      <i val="1"/>
+      <sz val="12"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <charset val="204"/>
+      <family val="2"/>
+      <sz val="12"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <charset val="204"/>
+      <family val="2"/>
+      <i val="1"/>
+      <sz val="13"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <charset val="204"/>
+      <family val="2"/>
+      <sz val="13"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <charset val="204"/>
+      <family val="2"/>
+      <i val="1"/>
+      <sz val="14"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <charset val="204"/>
+      <family val="2"/>
+      <sz val="14"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <charset val="204"/>
+      <family val="2"/>
+      <i val="1"/>
+      <sz val="15"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <charset val="204"/>
+      <family val="2"/>
+      <sz val="15"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <charset val="204"/>
+      <family val="2"/>
+      <i val="1"/>
+      <sz val="16"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <charset val="204"/>
+      <family val="2"/>
+      <sz val="16"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <charset val="204"/>
+      <family val="2"/>
+      <i val="1"/>
+      <sz val="17"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <charset val="204"/>
+      <family val="2"/>
+      <sz val="17"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <charset val="204"/>
+      <family val="2"/>
+      <i val="1"/>
+      <sz val="6"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <charset val="204"/>
+      <family val="2"/>
+      <sz val="6"/>
     </font>
   </fonts>
   <fills count="2">
@@ -71,12 +252,48 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -444,166 +661,218 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
+  <sheetPr filterMode="0">
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
+    <pageSetUpPr fitToPage="0"/>
   </sheetPr>
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.55078125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B1" s="2" t="inlineStr">
+    <row r="1" ht="15" customHeight="1" s="5">
+      <c r="A1" s="6" t="inlineStr">
+        <is>
+          <t>000faf0sa</t>
+        </is>
+      </c>
+      <c r="B1" s="7" t="inlineStr">
         <is>
           <t>123</t>
         </is>
       </c>
-      <c r="C1" s="2" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="inlineStr">
+      <c r="C1" s="7" t="inlineStr">
+        <is>
+          <t>opopop</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="15" customHeight="1" s="5">
+      <c r="A2" s="10" t="inlineStr">
         <is>
           <t>f</t>
         </is>
       </c>
-      <c r="B2" s="2" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="C2" s="2" t="inlineStr">
+      <c r="B2" s="11" t="inlineStr">
+        <is>
+          <t>jajaja</t>
+        </is>
+      </c>
+      <c r="C2" s="7" t="inlineStr">
         <is>
           <t>afsaf</t>
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="2" t="inlineStr">
+    <row r="3" ht="15" customHeight="1" s="5">
+      <c r="A3" s="12" t="inlineStr">
         <is>
           <t>d</t>
         </is>
       </c>
-      <c r="B3" s="2" t="inlineStr">
+      <c r="B3" s="13" t="inlineStr">
         <is>
           <t>wqrw</t>
         </is>
       </c>
-      <c r="C3" s="2" t="inlineStr">
+      <c r="C3" s="14" t="inlineStr">
         <is>
           <t>ффф</t>
         </is>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="2" t="n">
+    <row r="4" ht="15" customHeight="1" s="5">
+      <c r="A4" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="B4" s="2" t="inlineStr">
-        <is>
-          <t>sgd</t>
-        </is>
-      </c>
-      <c r="C4" s="2" t="inlineStr">
-        <is>
-          <t>124</t>
+      <c r="B4" s="14" t="inlineStr">
+        <is>
+          <t>siuuu</t>
+        </is>
+      </c>
+      <c r="C4" s="14" t="inlineStr">
+        <is>
+          <t>124124214</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
+  <sheetPr filterMode="0">
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
+    <pageSetUpPr fitToPage="0"/>
   </sheetPr>
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.55078125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
+    <row r="1" ht="15" customHeight="1" s="5">
+      <c r="A1" s="6" t="inlineStr">
         <is>
           <t>124</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
+      <c r="C1" s="6" t="inlineStr">
+        <is>
+          <t>14124</t>
+        </is>
+      </c>
+      <c r="D1" s="6" t="inlineStr">
         <is>
           <t>1421</t>
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>124</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
+    <row r="2" ht="15" customHeight="1" s="5">
+      <c r="B2" s="9" t="inlineStr">
+        <is>
+          <t>124214124</t>
+        </is>
+      </c>
+      <c r="C2" s="6" t="inlineStr">
         <is>
           <t>afasa</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="D2" s="6" t="inlineStr">
         <is>
           <t>ewt</t>
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="C3" t="inlineStr">
+    <row r="3" ht="15" customHeight="1" s="5">
+      <c r="B3" s="6" t="inlineStr">
+        <is>
+          <t>gsdgsd</t>
+        </is>
+      </c>
+      <c r="C3" s="6" t="inlineStr">
         <is>
           <t>fsgsdg</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="D3" s="6" t="inlineStr">
         <is>
           <t>1512</t>
         </is>
       </c>
     </row>
-    <row r="4">
-      <c r="C4" t="n">
+    <row r="4" ht="12.8" customHeight="1" s="5">
+      <c r="A4" s="6" t="inlineStr">
+        <is>
+          <t>322</t>
+        </is>
+      </c>
+      <c r="C4" s="7" t="n">
         <v>124121</v>
       </c>
-    </row>
-    <row r="5">
-      <c r="C5" t="inlineStr">
+      <c r="D4" s="7" t="inlineStr">
+        <is>
+          <t>14124</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="12.8" customHeight="1" s="5">
+      <c r="A5" s="6" t="n"/>
+      <c r="C5" s="7" t="inlineStr">
         <is>
           <t>sgd</t>
         </is>
       </c>
-    </row>
-    <row r="6"/>
-    <row r="7">
-      <c r="D7" t="inlineStr">
+      <c r="D5" s="7" t="inlineStr">
+        <is>
+          <t>aooaoa</t>
+        </is>
+      </c>
+    </row>
+    <row r="6" ht="12.8" customHeight="1" s="5">
+      <c r="A6" s="8" t="inlineStr">
         <is>
           <t>aaaa</t>
         </is>
       </c>
+      <c r="B6" s="8" t="inlineStr"/>
+      <c r="D6" s="6" t="inlineStr">
+        <is>
+          <t>siuuuuuu</t>
+        </is>
+      </c>
+    </row>
+    <row r="7" ht="12.8" customHeight="1" s="5">
+      <c r="A7" s="8" t="inlineStr">
+        <is>
+          <t>da</t>
+        </is>
+      </c>
+      <c r="B7" s="8" t="n"/>
+      <c r="C7" s="6" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="D7" s="6" t="inlineStr">
+        <is>
+          <t>aaaa</t>
+        </is>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
 </worksheet>
 </file>
</xml_diff>